<commit_message>
Fix bug: not removing ID and TIME in features Rerun training and model assessment
</commit_message>
<xml_diff>
--- a/models/LogisticRegression_feature_importances.xlsx
+++ b/models/LogisticRegression_feature_importances.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.971893954434276</v>
+        <v>1.972867202374893</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.971893954434276</v>
+        <v>-1.972867202374893</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.970296184382253</v>
+        <v>1.971266631690917</v>
       </c>
       <c r="C3" t="n">
-        <v>1.970296184382253</v>
+        <v>1.971266631690917</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.877862659207737</v>
+        <v>1.878460343696272</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.877862659207737</v>
+        <v>-1.878460343696272</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.875870339751558</v>
+        <v>1.876466050243653</v>
       </c>
       <c r="C5" t="n">
-        <v>1.875870339751558</v>
+        <v>1.876466050243653</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.711050237094639</v>
+        <v>1.711722455031699</v>
       </c>
       <c r="C6" t="n">
-        <v>1.711050237094639</v>
+        <v>1.711722455031699</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.705088436619419</v>
+        <v>1.705760223294286</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.705088436619419</v>
+        <v>-1.705760223294286</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.665861800638249</v>
+        <v>1.666467294751642</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.665861800638249</v>
+        <v>-1.666467294751642</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.658885200404145</v>
+        <v>1.659492596044235</v>
       </c>
       <c r="C9" t="n">
-        <v>1.658885200404145</v>
+        <v>1.659492596044235</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.346446679487365</v>
+        <v>1.347239778896966</v>
       </c>
       <c r="C10" t="n">
-        <v>1.346446679487365</v>
+        <v>1.347239778896966</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.346207168457823</v>
+        <v>1.347000357052889</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.346207168457823</v>
+        <v>-1.347000357052889</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.254036521908684</v>
+        <v>1.254475242266157</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.254036521908684</v>
+        <v>-1.254475242266157</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.251718843634197</v>
+        <v>1.252158478164886</v>
       </c>
       <c r="C13" t="n">
-        <v>1.251718843634197</v>
+        <v>1.252158478164886</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.249387662045468</v>
+        <v>1.250186222938902</v>
       </c>
       <c r="C14" t="n">
-        <v>1.249387662045468</v>
+        <v>1.250186222938902</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.246056675469461</v>
+        <v>1.246855862823902</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.246056675469461</v>
+        <v>-1.246855862823902</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.159960590106963</v>
+        <v>1.160202461512431</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.159960590106963</v>
+        <v>-1.160202461512431</v>
       </c>
     </row>
     <row r="17">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.149628770966599</v>
+        <v>1.149869891247123</v>
       </c>
       <c r="C17" t="n">
-        <v>1.149628770966599</v>
+        <v>1.149869891247123</v>
       </c>
     </row>
     <row r="18">
@@ -665,10 +665,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.11354718946354</v>
+        <v>1.114194718010076</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.11354718946354</v>
+        <v>-1.114194718010076</v>
       </c>
     </row>
     <row r="19">
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.11175535483543</v>
+        <v>1.112403182527738</v>
       </c>
       <c r="C19" t="n">
-        <v>1.11175535483543</v>
+        <v>1.112403182527738</v>
       </c>
     </row>
     <row r="20">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.069244396455713</v>
+        <v>1.069885245401764</v>
       </c>
       <c r="C20" t="n">
-        <v>1.069244396455713</v>
+        <v>1.069885245401764</v>
       </c>
     </row>
     <row r="21">
@@ -704,10 +704,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.020557791483592</v>
+        <v>1.02160183504064</v>
       </c>
       <c r="C21" t="n">
-        <v>1.020557791483592</v>
+        <v>1.02160183504064</v>
       </c>
     </row>
     <row r="22">
@@ -717,10 +717,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.007585582022267</v>
+        <v>1.008630107904062</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.007585582022267</v>
+        <v>-1.008630107904062</v>
       </c>
     </row>
     <row r="23">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.003851662804168</v>
+        <v>1.003527321239619</v>
       </c>
       <c r="C23" t="n">
-        <v>1.003851662804168</v>
+        <v>1.003527321239619</v>
       </c>
     </row>
     <row r="24">
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.991590250863345</v>
+        <v>0.9912640850371018</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.991590250863345</v>
+        <v>-0.9912640850371018</v>
       </c>
     </row>
     <row r="25">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9852801168412085</v>
+        <v>0.9857034989990721</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9852801168412085</v>
+        <v>0.9857034989990721</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9491052968205669</v>
+        <v>0.9490226336024571</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.9491052968205669</v>
+        <v>-0.9490226336024571</v>
       </c>
     </row>
     <row r="27">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.938637800948675</v>
+        <v>0.9385550747022456</v>
       </c>
       <c r="C27" t="n">
-        <v>0.938637800948675</v>
+        <v>0.9385550747022456</v>
       </c>
     </row>
     <row r="28">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.9037607486921213</v>
+        <v>0.9043446853245833</v>
       </c>
       <c r="C28" t="n">
-        <v>0.9037607486921213</v>
+        <v>0.9043446853245833</v>
       </c>
     </row>
     <row r="29">
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8975351984407918</v>
+        <v>0.8981198747201898</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8975351984407918</v>
+        <v>-0.8981198747201898</v>
       </c>
     </row>
     <row r="30">
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.8379618535688753</v>
+        <v>0.8381534343579177</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.8379618535688753</v>
+        <v>-0.8381534343579177</v>
       </c>
     </row>
     <row r="31">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.8239361525232104</v>
+        <v>0.8241306187908757</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8239361525232104</v>
+        <v>0.8241306187908757</v>
       </c>
     </row>
     <row r="32">
@@ -847,10 +847,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.7540307482289136</v>
+        <v>0.7539077161022443</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7540307482289136</v>
+        <v>0.7539077161022443</v>
       </c>
     </row>
     <row r="33">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.7526401284361403</v>
+        <v>0.752516268852252</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.7526401284361403</v>
+        <v>-0.752516268852252</v>
       </c>
     </row>
     <row r="34">
@@ -873,10 +873,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.7350834672448788</v>
+        <v>0.735110797969498</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.7350834672448788</v>
+        <v>-0.735110797969498</v>
       </c>
     </row>
     <row r="35">
@@ -886,10 +886,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.7292297008645671</v>
+        <v>0.7292560578262479</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7292297008645671</v>
+        <v>0.7292560578262479</v>
       </c>
     </row>
     <row r="36">
@@ -899,10 +899,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.7180434871301106</v>
+        <v>0.7178408600855275</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.7180434871301106</v>
+        <v>-0.7178408600855275</v>
       </c>
     </row>
     <row r="37">
@@ -912,10 +912,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.7132575565423155</v>
+        <v>0.7130565062589005</v>
       </c>
       <c r="C37" t="n">
-        <v>0.7132575565423155</v>
+        <v>0.7130565062589005</v>
       </c>
     </row>
     <row r="38">
@@ -925,10 +925,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.6813177531241381</v>
+        <v>0.6819595679567425</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.6813177531241381</v>
+        <v>-0.6819595679567425</v>
       </c>
     </row>
     <row r="39">
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.669654827970679</v>
+        <v>0.6697698805372652</v>
       </c>
       <c r="C39" t="n">
-        <v>0.669654827970679</v>
+        <v>0.6697698805372652</v>
       </c>
     </row>
     <row r="40">
@@ -951,10 +951,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.6638716937882103</v>
+        <v>0.6639868535600477</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.6638716937882103</v>
+        <v>-0.6639868535600477</v>
       </c>
     </row>
     <row r="41">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.6278162494264455</v>
+        <v>0.6278098002294416</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.6278162494264455</v>
+        <v>-0.6278098002294416</v>
       </c>
     </row>
     <row r="42">
@@ -977,10 +977,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.6230048504018191</v>
+        <v>0.6231706036827964</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.6230048504018191</v>
+        <v>-0.6231706036827964</v>
       </c>
     </row>
     <row r="43">
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.6215560393630827</v>
+        <v>0.6216686731586589</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6215560393630827</v>
+        <v>0.6216686731586589</v>
       </c>
     </row>
     <row r="44">
@@ -1003,10 +1003,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.6159174948391023</v>
+        <v>0.6160292075661719</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.6159174948391023</v>
+        <v>-0.6160292075661719</v>
       </c>
     </row>
     <row r="45">
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6141701943022179</v>
+        <v>0.6143352796792046</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6141701943022179</v>
+        <v>0.6143352796792046</v>
       </c>
     </row>
     <row r="46">
@@ -1029,10 +1029,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.6014438951199214</v>
+        <v>0.6014448571174996</v>
       </c>
       <c r="C46" t="n">
-        <v>0.6014438951199214</v>
+        <v>0.6014448571174996</v>
       </c>
     </row>
     <row r="47">
@@ -1042,10 +1042,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.5916556804997961</v>
+        <v>0.5917138277664491</v>
       </c>
       <c r="C47" t="n">
-        <v>0.5916556804997961</v>
+        <v>0.5917138277664491</v>
       </c>
     </row>
     <row r="48">
@@ -1055,10 +1055,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.5843107638941636</v>
+        <v>0.5844352341549742</v>
       </c>
       <c r="C48" t="n">
-        <v>0.5843107638941636</v>
+        <v>0.5844352341549742</v>
       </c>
     </row>
     <row r="49">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.5824361933683699</v>
+        <v>0.5824969255029668</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.5824361933683699</v>
+        <v>-0.5824969255029668</v>
       </c>
     </row>
     <row r="50">
@@ -1081,10 +1081,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.5618540654583197</v>
+        <v>0.5618641816389968</v>
       </c>
       <c r="C50" t="n">
-        <v>0.5618540654583197</v>
+        <v>0.5618641816389968</v>
       </c>
     </row>
     <row r="51">
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.5618540654583197</v>
+        <v>0.5618641816389968</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.5618540654583197</v>
+        <v>-0.5618641816389968</v>
       </c>
     </row>
     <row r="52">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.5093577427697303</v>
+        <v>0.5092927852142224</v>
       </c>
       <c r="C52" t="n">
-        <v>0.5093577427697303</v>
+        <v>0.5092927852142224</v>
       </c>
     </row>
     <row r="53">
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.5004604169895848</v>
+        <v>0.5003962368892488</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.5004604169895848</v>
+        <v>-0.5003962368892488</v>
       </c>
     </row>
     <row r="54">
@@ -1133,10 +1133,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.4538417755787685</v>
+        <v>0.4538522834820553</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.4538417755787685</v>
+        <v>-0.4538522834820553</v>
       </c>
     </row>
     <row r="55">
@@ -1146,10 +1146,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.452162920739169</v>
+        <v>0.4527351436223263</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.452162920739169</v>
+        <v>-0.4527351436223263</v>
       </c>
     </row>
     <row r="56">
@@ -1159,10 +1159,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.4456717341561303</v>
+        <v>0.4459628754566192</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.4456717341561303</v>
+        <v>-0.4459628754566192</v>
       </c>
     </row>
     <row r="57">
@@ -1172,10 +1172,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.4389022513500316</v>
+        <v>0.4394745195813375</v>
       </c>
       <c r="C57" t="n">
-        <v>0.4389022513500316</v>
+        <v>0.4394745195813375</v>
       </c>
     </row>
     <row r="58">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.4337811339997808</v>
+        <v>0.4340748167165208</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4337811339997808</v>
+        <v>0.4340748167165208</v>
       </c>
     </row>
     <row r="59">
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.4289381349156913</v>
+        <v>0.4290963839474641</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.4289381349156913</v>
+        <v>-0.4290963839474641</v>
       </c>
     </row>
     <row r="60">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.4271710869078633</v>
+        <v>0.4273290704760714</v>
       </c>
       <c r="C60" t="n">
-        <v>0.4271710869078633</v>
+        <v>0.4273290704760714</v>
       </c>
     </row>
     <row r="61">
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.397241536759054</v>
+        <v>0.3972231697560624</v>
       </c>
       <c r="C61" t="n">
-        <v>0.397241536759054</v>
+        <v>0.3972231697560624</v>
       </c>
     </row>
     <row r="62">
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.3958641254457896</v>
+        <v>0.3963320849269483</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3958641254457896</v>
+        <v>0.3963320849269483</v>
       </c>
     </row>
     <row r="63">
@@ -1250,10 +1250,10 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.3889010265746224</v>
+        <v>0.3888820508079136</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.3889010265746224</v>
+        <v>-0.3888820508079136</v>
       </c>
     </row>
     <row r="64">
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.3879956150878878</v>
+        <v>0.3884650075334233</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.3879956150878878</v>
+        <v>-0.3884650075334233</v>
       </c>
     </row>
     <row r="65">
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.3798361630981957</v>
+        <v>0.3799393940476218</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.3798361630981957</v>
+        <v>-0.3799393940476218</v>
       </c>
     </row>
     <row r="66">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.3647748386463073</v>
+        <v>0.3648779972671397</v>
       </c>
       <c r="C66" t="n">
-        <v>0.3647748386463073</v>
+        <v>0.3648779972671397</v>
       </c>
     </row>
     <row r="67">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.3621671247093023</v>
+        <v>0.3625654406160402</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.3621671247093023</v>
+        <v>-0.3625654406160402</v>
       </c>
     </row>
     <row r="68">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.3588506772214579</v>
+        <v>0.3592474067357506</v>
       </c>
       <c r="C68" t="n">
-        <v>0.3588506772214579</v>
+        <v>0.3592474067357506</v>
       </c>
     </row>
     <row r="69">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.330165526711046</v>
+        <v>0.3305932266251619</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.330165526711046</v>
+        <v>-0.3305932266251619</v>
       </c>
     </row>
     <row r="70">
@@ -1341,10 +1341,10 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.2742237254283572</v>
+        <v>0.2742304582254372</v>
       </c>
       <c r="C70" t="n">
-        <v>0.2742237254283572</v>
+        <v>0.2742304582254372</v>
       </c>
     </row>
     <row r="71">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.2691848953106033</v>
+        <v>0.2692701445749445</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.2691848953106033</v>
+        <v>-0.2692701445749445</v>
       </c>
     </row>
     <row r="72">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.2596380565230948</v>
+        <v>0.2597235079340913</v>
       </c>
       <c r="C72" t="n">
-        <v>0.2596380565230948</v>
+        <v>0.2597235079340913</v>
       </c>
     </row>
     <row r="73">
@@ -1380,10 +1380,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2455973234951504</v>
+        <v>0.2456697249782782</v>
       </c>
       <c r="C73" t="n">
-        <v>0.2455973234951504</v>
+        <v>0.2456697249782782</v>
       </c>
     </row>
     <row r="74">
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.2334837881634935</v>
+        <v>0.2335582782641035</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.2334837881634935</v>
+        <v>-0.2335582782641035</v>
       </c>
     </row>
     <row r="75">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.2229648280822568</v>
+        <v>0.2224650746959</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.2229648280822568</v>
+        <v>-0.2224650746959</v>
       </c>
     </row>
     <row r="76">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.2214591639230328</v>
+        <v>0.2209614849489828</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2214591639230328</v>
+        <v>0.2209614849489828</v>
       </c>
     </row>
     <row r="77">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.2175209249283663</v>
+        <v>0.2175294261958693</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.2175209249283663</v>
+        <v>-0.2175294261958693</v>
       </c>
     </row>
     <row r="78">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.2150099266680976</v>
+        <v>0.2150177212267913</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.2150099266680976</v>
+        <v>-0.2150177212267913</v>
       </c>
     </row>
     <row r="79">
@@ -1458,10 +1458,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.2117545263966765</v>
+        <v>0.2117630424375003</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.2117545263966765</v>
+        <v>-0.2117630424375003</v>
       </c>
     </row>
     <row r="80">
@@ -1471,244 +1471,244 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.2095968347630554</v>
+        <v>0.2096048283728223</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.2095968347630554</v>
+        <v>-0.2096048283728223</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_4</t>
+          <t>NUMERICAL_1</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.2060340201547475</v>
+        <v>0.1865699568957469</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2060340201547475</v>
+        <v>-0.1865699568957469</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_1</t>
+          <t>NUMERICAL_33</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.186755169416589</v>
+        <v>0.1862217390326682</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.186755169416589</v>
+        <v>0.1862217390326682</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_33</t>
+          <t>NUMERICAL_33_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.1859646473571956</v>
+        <v>0.1804389322857882</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1859646473571956</v>
+        <v>-0.1804389322857882</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_33_std_dev_last_30_days</t>
+          <t>CATEGORICAL_1_value_FCOHQ</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.1801805331243415</v>
+        <v>0.1791085776735963</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.1801805331243415</v>
+        <v>0.1791085776735963</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_1_value_FCOHQ</t>
+          <t>NUMERICAL_1_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.1791048138725111</v>
+        <v>0.1754351193164419</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1791048138725111</v>
+        <v>0.1754351193164419</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_1_std_dev_last_30_days</t>
+          <t>NUMERICAL_0</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.1756198188927522</v>
+        <v>0.1633573235391143</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1756198188927522</v>
+        <v>0.1633573235391143</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_0</t>
+          <t>NUMERICAL_0_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.1631922670063115</v>
+        <v>0.1534895112681541</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1631922670063115</v>
+        <v>-0.1534895112681541</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_0_std_dev_last_30_days</t>
+          <t>CATEGORICAL_4_value_JK</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.1533228402631027</v>
+        <v>0.1517322805563497</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.1533228402631027</v>
+        <v>0.1517322805563497</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_4_value_JK</t>
+          <t>CATEGORICAL_2_value_AB</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.1517327583478557</v>
+        <v>0.148528432444057</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1517327583478557</v>
+        <v>0.148528432444057</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_2_value_AB</t>
+          <t>CATEGORICAL_5_value_WE</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.1485296310023788</v>
+        <v>0.1456144342492815</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1485296310023788</v>
+        <v>0.1456144342492815</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_5_value_WE</t>
+          <t>CATEGORICAL_3_value_DF</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.1456149048186428</v>
+        <v>0.1430319639467789</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1456149048186428</v>
+        <v>0.1430319639467789</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_3_value_DF</t>
+          <t>MONTH_APPLICATION_value_4</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.1430329655750166</v>
+        <v>0.1429576498229529</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1430329655750166</v>
+        <v>0.1429576498229529</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>ID_APPLICATION</t>
+          <t>NUMERICAL_30_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.1318075235444907</v>
+        <v>0.115738025978838</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.1318075235444907</v>
+        <v>-0.115738025978838</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_30_std_dev_last_30_days</t>
+          <t>NUMERICAL_27_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.1156115630305837</v>
+        <v>0.1116853756200428</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.1156115630305837</v>
+        <v>0.1116853756200428</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_27_std_dev_last_30_days</t>
+          <t>NUMERICAL_27</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.1110247670305845</v>
+        <v>0.1019126342553063</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1110247670305845</v>
+        <v>-0.1019126342553063</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_27</t>
+          <t>CATEGORICAL_5_value_unkown</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.1012514168886684</v>
+        <v>0.06196539284892139</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.1012514168886684</v>
+        <v>0.06196539284892139</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_8</t>
+          <t>CATEGORICAL_2_value_unkown</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.0757438390550224</v>
+        <v>0.06196539284892139</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.0757438390550224</v>
+        <v>0.06196539284892139</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_2_value_unkown</t>
+          <t>CATEGORICAL_4_value_unkown</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.06196539284892139</v>
       </c>
       <c r="C98" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.06196539284892139</v>
       </c>
     </row>
     <row r="99">
@@ -1718,36 +1718,36 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.06196539284892139</v>
       </c>
       <c r="C99" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.06196539284892139</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_4_value_unkown</t>
+          <t>CATEGORICAL_7_value_B</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.05777140100133461</v>
       </c>
       <c r="C100" t="n">
-        <v>0.06195698220203791</v>
+        <v>-0.05777140100133461</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_5_value_unkown</t>
+          <t>NUMERICAL_26_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.06195698220203791</v>
+        <v>0.03847486441576235</v>
       </c>
       <c r="C101" t="n">
-        <v>0.06195698220203791</v>
+        <v>-0.03847486441576235</v>
       </c>
     </row>
     <row r="102">
@@ -1757,322 +1757,322 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.05999405354915183</v>
+        <v>0.03344204937114987</v>
       </c>
       <c r="C102" t="n">
-        <v>-0.05999405354915183</v>
+        <v>-0.03344204937114987</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_7</t>
+          <t>MONTH_APPLICATION_value_11</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.05811255359754598</v>
+        <v>0.03246069841469804</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.05811255359754598</v>
+        <v>-0.03246069841469804</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_7_value_B</t>
+          <t>CATEGORICAL_8_value_BB</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.05776387881971692</v>
+        <v>0.03195790575928951</v>
       </c>
       <c r="C104" t="n">
-        <v>-0.05776387881971692</v>
+        <v>-0.03195790575928951</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_3</t>
+          <t>CATEGORICAL_8_value_AA</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.04776215607924813</v>
+        <v>0.03195790575923354</v>
       </c>
       <c r="C105" t="n">
-        <v>0.04776215607924813</v>
+        <v>0.03195790575923354</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_11</t>
+          <t>MONTH_APPLICATION_value_12</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.04343515546468898</v>
+        <v>0.02883134919428099</v>
       </c>
       <c r="C106" t="n">
-        <v>-0.04343515546468898</v>
+        <v>-0.02883134919428099</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_9</t>
+          <t>NUMERICAL_26</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.04182351439875026</v>
+        <v>0.02765454943582196</v>
       </c>
       <c r="C107" t="n">
-        <v>-0.04182351439875026</v>
+        <v>0.02765454943582196</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_26_std_dev_last_30_days</t>
+          <t>CATEGORICAL_6_value_A</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.03834569599438788</v>
+        <v>0.02241054816895291</v>
       </c>
       <c r="C108" t="n">
-        <v>-0.03834569599438788</v>
+        <v>0.02241054816895291</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_8_value_BB</t>
+          <t>DAY_APPLICATION_value_26</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.03195948710940864</v>
+        <v>0.02086763077713635</v>
       </c>
       <c r="C109" t="n">
-        <v>-0.03195948710940864</v>
+        <v>0.02086763077713635</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_8_value_AA</t>
+          <t>DAY_APPLICATION_value_20</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.03195948710940045</v>
+        <v>0.01882588606905898</v>
       </c>
       <c r="C110" t="n">
-        <v>0.03195948710940045</v>
+        <v>0.01882588606905898</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_26</t>
+          <t>MONTH_APPLICATION_value_8</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.0275248956493982</v>
+        <v>0.01851206534126017</v>
       </c>
       <c r="C111" t="n">
-        <v>0.0275248956493982</v>
+        <v>-0.01851206534126017</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_12</t>
+          <t>DAY_APPLICATION_value_7</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.02508053070109484</v>
+        <v>0.01674489274354554</v>
       </c>
       <c r="C112" t="n">
-        <v>-0.02508053070109484</v>
+        <v>-0.01674489274354554</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_26</t>
+          <t>MONTH_APPLICATION_value_2</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.02377832683005172</v>
+        <v>0.01605152028203273</v>
       </c>
       <c r="C113" t="n">
-        <v>0.02377832683005172</v>
+        <v>-0.01605152028203273</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_6_value_A</t>
+          <t>DAY_APPLICATION_value_18</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.02237637586857134</v>
+        <v>0.01488588199829113</v>
       </c>
       <c r="C114" t="n">
-        <v>0.02237637586857134</v>
+        <v>-0.01488588199829113</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_20</t>
+          <t>DAY_APPLICATION_value_15</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.01998108317214759</v>
+        <v>0.01479444755104834</v>
       </c>
       <c r="C115" t="n">
-        <v>0.01998108317214759</v>
+        <v>-0.01479444755104834</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_7</t>
+          <t>CATEGORICAL_0_value_SUPSY</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.01930215459138498</v>
+        <v>0.01438254591533904</v>
       </c>
       <c r="C116" t="n">
-        <v>-0.01930215459138498</v>
+        <v>0.01438254591533904</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_27</t>
+          <t>CATEGORICAL_6_value_C</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.01710285124348001</v>
+        <v>0.01423029093649983</v>
       </c>
       <c r="C117" t="n">
-        <v>0.01710285124348001</v>
+        <v>-0.01423029093649983</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_2</t>
+          <t>DAY_APPLICATION_value_27</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.01706340981269009</v>
+        <v>0.01389489668370205</v>
       </c>
       <c r="C118" t="n">
-        <v>0.01706340981269009</v>
+        <v>0.01389489668370205</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_28</t>
+          <t>DAY_APPLICATION_value_10</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.01665849510691813</v>
+        <v>0.01340163703762189</v>
       </c>
       <c r="C119" t="n">
-        <v>0.01665849510691813</v>
+        <v>-0.01340163703762189</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>MONTH_APPLICATION_value_1</t>
+          <t>DAY_APPLICATION_value_28</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.01550602201270145</v>
+        <v>0.01312878728968315</v>
       </c>
       <c r="C120" t="n">
-        <v>0.01550602201270145</v>
+        <v>0.01312878728968315</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_10</t>
+          <t>DAY_APPLICATION_value_22</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.01511269264711137</v>
+        <v>0.01263617083263885</v>
       </c>
       <c r="C121" t="n">
-        <v>-0.01511269264711137</v>
+        <v>0.01263617083263885</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_15</t>
+          <t>DOW_APPLICATION_value_6</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.01509624151208312</v>
+        <v>0.01144724018516868</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.01509624151208312</v>
+        <v>0.01144724018516868</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_0_value_SUPSY</t>
+          <t>MONTH_APPLICATION_value_7</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.01438246481107595</v>
+        <v>0.01134447957979535</v>
       </c>
       <c r="C123" t="n">
-        <v>0.01438246481107595</v>
+        <v>-0.01134447957979535</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_22</t>
+          <t>DAY_APPLICATION_value_19</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.01437285860494208</v>
+        <v>0.01059549047665766</v>
       </c>
       <c r="C124" t="n">
-        <v>0.01437285860494208</v>
+        <v>0.01059549047665766</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_18</t>
+          <t>DAY_APPLICATION_value_23</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.01434809186592529</v>
+        <v>0.01032194048784713</v>
       </c>
       <c r="C125" t="n">
-        <v>-0.01434809186592529</v>
+        <v>0.01032194048784713</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_6_value_C</t>
+          <t>CATEGORICAL_6_value_B</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.01420605726582745</v>
+        <v>0.01024098103359272</v>
       </c>
       <c r="C126" t="n">
-        <v>-0.01420605726582745</v>
+        <v>-0.01024098103359272</v>
       </c>
     </row>
     <row r="127">
@@ -2082,296 +2082,296 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.01333841412099553</v>
+        <v>0.009673989907537033</v>
       </c>
       <c r="C127" t="n">
-        <v>-0.01333841412099553</v>
+        <v>-0.009673989907537033</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_30</t>
+          <t>DAY_APPLICATION_value_17</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.01248680473145413</v>
+        <v>0.009551418273577939</v>
       </c>
       <c r="C128" t="n">
-        <v>0.01248680473145413</v>
+        <v>-0.009551418273577939</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_23</t>
+          <t>CATEGORICAL_0_value_JJUFY</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.01235507615761721</v>
+        <v>0.008708396945942956</v>
       </c>
       <c r="C129" t="n">
-        <v>0.01235507615761721</v>
+        <v>-0.008708396945942956</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_6</t>
+          <t>DAY_APPLICATION_value_30</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.01144852228389355</v>
+        <v>0.008568810430973879</v>
       </c>
       <c r="C130" t="n">
-        <v>0.01144852228389355</v>
+        <v>0.008568810430973879</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_19</t>
+          <t>HOUR_APPLICATION</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.01141603585211817</v>
+        <v>0.008543025478490614</v>
       </c>
       <c r="C131" t="n">
-        <v>0.01141603585211817</v>
+        <v>0.008543025478490614</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_5</t>
+          <t>NUMERICAL_2</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.01062637838449503</v>
+        <v>0.007885009333720404</v>
       </c>
       <c r="C132" t="n">
-        <v>-0.01062637838449503</v>
+        <v>0.007885009333720404</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_6_value_B</t>
+          <t>DAY_APPLICATION_value_12</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.01022789625106598</v>
+        <v>0.007524565653084275</v>
       </c>
       <c r="C133" t="n">
-        <v>-0.01022789625106598</v>
+        <v>-0.007524565653084275</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_2</t>
+          <t>DAY_APPLICATION_value_5</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.009866160634314274</v>
+        <v>0.007488313344923793</v>
       </c>
       <c r="C134" t="n">
-        <v>-0.009866160634314274</v>
+        <v>-0.007488313344923793</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_29</t>
+          <t>DAY_APPLICATION_value_16</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.009382121461237151</v>
+        <v>0.007308927535851692</v>
       </c>
       <c r="C135" t="n">
-        <v>0.009382121461237151</v>
+        <v>-0.007308927535851692</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_17</t>
+          <t>DOW_APPLICATION_value_5</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.00929469285374851</v>
+        <v>0.007210241773926858</v>
       </c>
       <c r="C136" t="n">
-        <v>-0.00929469285374851</v>
+        <v>-0.007210241773926858</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_6</t>
+          <t>NUMERICAL_2_std_dev_last_30_days</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.009240196734585277</v>
+        <v>0.00715661846311132</v>
       </c>
       <c r="C137" t="n">
-        <v>-0.009240196734585277</v>
+        <v>-0.00715661846311132</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>HOUR_APPLICATION</t>
+          <t>DAY_APPLICATION_value_6</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.009003536196312955</v>
+        <v>0.006392529581572086</v>
       </c>
       <c r="C138" t="n">
-        <v>0.009003536196312955</v>
+        <v>-0.006392529581572086</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_0_value_JJUFY</t>
+          <t>DAY_APPLICATION_value_25</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.008707950647168602</v>
+        <v>0.006010291200453858</v>
       </c>
       <c r="C139" t="n">
-        <v>-0.008707950647168602</v>
+        <v>0.006010291200453858</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_12</t>
+          <t>DAY_APPLICATION_value_2</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.008661326175125548</v>
+        <v>0.005932472227481251</v>
       </c>
       <c r="C140" t="n">
-        <v>-0.008661326175125548</v>
+        <v>-0.005932472227481251</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_25</t>
+          <t>DAY_APPLICATION_value_29</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.008643212779597636</v>
+        <v>0.005764044699607888</v>
       </c>
       <c r="C141" t="n">
-        <v>0.008643212779597636</v>
+        <v>0.005764044699607888</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_4</t>
+          <t>DAY_APPLICATION_value_24</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.008360218361811084</v>
+        <v>0.005680248066891133</v>
       </c>
       <c r="C142" t="n">
-        <v>-0.008360218361811084</v>
+        <v>0.005680248066891133</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_24</t>
+          <t>DAY_APPLICATION_value_9</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.008011590951246372</v>
+        <v>0.005378238832675145</v>
       </c>
       <c r="C143" t="n">
-        <v>0.008011590951246372</v>
+        <v>0.005378238832675145</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_2</t>
+          <t>DAY_APPLICATION_value_8</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.00755774464453396</v>
+        <v>0.005155756922577906</v>
       </c>
       <c r="C144" t="n">
-        <v>0.00755774464453396</v>
+        <v>-0.005155756922577906</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_8</t>
+          <t>DAY_APPLICATION_value_4</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.007415821739399923</v>
+        <v>0.004956650993975522</v>
       </c>
       <c r="C145" t="n">
-        <v>-0.007415821739399923</v>
+        <v>-0.004956650993975522</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_16</t>
+          <t>CATEGORICAL_10_value_HNPAK</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.007334136276444224</v>
+        <v>0.004598471426060876</v>
       </c>
       <c r="C146" t="n">
-        <v>-0.007334136276444224</v>
+        <v>-0.004598471426060876</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_5</t>
+          <t>CATEGORICAL_10_value_NFAYV</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.007206624250767311</v>
+        <v>0.004598471425962375</v>
       </c>
       <c r="C147" t="n">
-        <v>-0.007206624250767311</v>
+        <v>0.004598471425962375</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>NUMERICAL_2_std_dev_last_30_days</t>
+          <t>CATEGORICAL_0_value_IMFRD</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.006831445519503237</v>
+        <v>0.004365475699838027</v>
       </c>
       <c r="C148" t="n">
-        <v>-0.006831445519503237</v>
+        <v>-0.004365475699838027</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_1</t>
+          <t>DOW_APPLICATION_value_1</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.006469461981963174</v>
+        <v>0.004051234894245501</v>
       </c>
       <c r="C149" t="n">
-        <v>-0.006469461981963174</v>
+        <v>-0.004051234894245501</v>
       </c>
     </row>
     <row r="150">
@@ -2381,217 +2381,204 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.005143563024170657</v>
+        <v>0.003725785357264679</v>
       </c>
       <c r="C150" t="n">
-        <v>-0.005143563024170657</v>
+        <v>-0.003725785357264679</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_31</t>
+          <t>MONTH_APPLICATION_value_1</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.004825099939371635</v>
+        <v>0.003656245755848129</v>
       </c>
       <c r="C151" t="n">
-        <v>0.004825099939371635</v>
+        <v>-0.003656245755848129</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_10_value_NFAYV</t>
+          <t>DAY_APPLICATION_value_13</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.004598912139935516</v>
+        <v>0.003234766395084579</v>
       </c>
       <c r="C152" t="n">
-        <v>0.004598912139935516</v>
+        <v>-0.003234766395084579</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_10_value_HNPAK</t>
+          <t>DOW_APPLICATION_value_3</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.004598912139933016</v>
+        <v>0.003024219403491201</v>
       </c>
       <c r="C153" t="n">
-        <v>-0.004598912139933016</v>
+        <v>-0.003024219403491201</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_0_value_IMFRD</t>
+          <t>CATEGORICAL_0_value_UQPEF</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.00436544141553903</v>
+        <v>0.002923323083193266</v>
       </c>
       <c r="C154" t="n">
-        <v>-0.00436544141553903</v>
+        <v>-0.002923323083193266</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_13</t>
+          <t>DAY_APPLICATION_value_21</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.004099246043908076</v>
+        <v>0.002748099668332766</v>
       </c>
       <c r="C155" t="n">
-        <v>-0.004099246043908076</v>
+        <v>-0.002748099668332766</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_1</t>
+          <t>DOW_APPLICATION_value_2</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.004050452450609047</v>
+        <v>0.002587760261459345</v>
       </c>
       <c r="C156" t="n">
-        <v>-0.004050452450609047</v>
+        <v>0.002587760261459345</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_9</t>
+          <t>DAY_APPLICATION_value_1</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.003384384654308007</v>
+        <v>0.002266296641735492</v>
       </c>
       <c r="C157" t="n">
-        <v>0.003384384654308007</v>
+        <v>-0.002266296641735492</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_3</t>
+          <t>DAY_APPLICATION_value_14</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.003028705787687584</v>
+        <v>0.001993389163858855</v>
       </c>
       <c r="C158" t="n">
-        <v>-0.003028705787687584</v>
+        <v>-0.001993389163858855</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_0_value_UQPEF</t>
+          <t>CATEGORICAL_0_value_FPTCW</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.002923364424386009</v>
+        <v>0.001596515774430793</v>
       </c>
       <c r="C159" t="n">
-        <v>-0.002923364424386009</v>
+        <v>0.001596515774430793</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_14</t>
+          <t>DAY_APPLICATION_value_31</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.002585452463135508</v>
+        <v>0.001398359526982454</v>
       </c>
       <c r="C160" t="n">
-        <v>-0.002585452463135508</v>
+        <v>0.001398359526982454</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_2</t>
+          <t>MONTH_APPLICATION_value_3</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.002585034995568356</v>
+        <v>0.0009600351551152781</v>
       </c>
       <c r="C161" t="n">
-        <v>0.002585034995568356</v>
+        <v>-0.0009600351551152781</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>CATEGORICAL_0_value_FPTCW</t>
+          <t>MONTH_APPLICATION_value_9</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.001596157216051288</v>
+        <v>0.0006891366379682177</v>
       </c>
       <c r="C162" t="n">
-        <v>0.001596157216051288</v>
+        <v>-0.0006891366379682177</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>DAY_APPLICATION_value_21</t>
+          <t>DOW_APPLICATION_value_4</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.001298059824537305</v>
+        <v>0.0002945708852986902</v>
       </c>
       <c r="C163" t="n">
-        <v>-0.001298059824537305</v>
+        <v>0.0002945708852986902</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_4</t>
+          <t>DOW_APPLICATION_value_0</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.0002940335106700715</v>
+        <v>0.0001101505862857624</v>
       </c>
       <c r="C164" t="n">
-        <v>0.0002940335106700715</v>
+        <v>-0.0001101505862857624</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>DOW_APPLICATION_value_0</t>
+          <t>MONTH_APPLICATION_value_5</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.000108046482313669</v>
+        <v>0</v>
       </c>
       <c r="C165" t="n">
-        <v>-0.000108046482313669</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="inlineStr">
-        <is>
-          <t>MONTH_APPLICATION_value_5</t>
-        </is>
-      </c>
-      <c r="B166" t="n">
-        <v>0</v>
-      </c>
-      <c r="C166" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>